<commit_message>
增加绳索功能, AOI, PerlinNoise, MarchingCubes
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/AnimatorStateConfig.xlsx
+++ b/Unity/Assets/Config/Excel/AnimatorStateConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToolSoft\U3D\Project\ETs\ET-OWDemo-1\Unity\Assets\Config\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\ET-OWDemo\Unity\Assets\Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB245946-4DCD-4F61-BC33-5A38CBDDDBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970B3225-2717-4F86-8250-5EFE6A1749AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AnimatorStateConfig" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -501,17 +501,17 @@
   <dimension ref="C3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="C10:E10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
@@ -608,7 +608,9 @@
       <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2">

</xml_diff>